<commit_message>
update few shot examples
</commit_message>
<xml_diff>
--- a/data/gpt_examples/Cardio.xlsx
+++ b/data/gpt_examples/Cardio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beimn\Documents\workdir\twelve-educational\logistic-regression\data\gpt_examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beimn\Documents\workdir\wordalization-logistic-regression\data\gpt_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1209BBC-2120-4D12-9921-C538EA68D863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CB880D-377A-4272-823E-5FDB7A10372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7680" yWindow="-11640" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>user</t>
   </si>
@@ -28,29 +28,35 @@
     <t>assistant</t>
   </si>
   <si>
-    <t>An age of 46 implies a moderately reduced risk of developing cardio issues. Being male implies no significant effect of developing cardio issues.A body mass index of 37.86 implies a strongly increased risk of developing cardio issues.A systolic blood pressure of 120 implies a moderately reduced risk of developing cardio issues.A diastolic blood pressure of 80 implies a moderately reduced risk of developing cardio issues. Having normal cholestero levels implies a strongly reduced risk of developing cardio issues. Having normal glucose levels implies a moderately reduced risk of developing cardio issues. Not smoking implies a moderately reduced risk of developing cardio issues. Not drinking alcohol implies a strongly reduced risk of developing cardio issues. Not having an active lifestyle implies a moderately increased risk of developing cardio issues. The patient's overall risk of developing cardio issues is average compared to other patients who come into the clinic.</t>
+    <t>An age of 50 implies no significant effect of developing cardio issues. Being male implies no significant effect of developing cardio issues. Being male increases your risk age by 1.61 years. A body mass index of 21.97 implies no significant effect of developing cardio issues.A body mass index of 21.97 decreases your risk age by 3.6 years. A systolic blood pressure of 110 implies a strongly reduced risk of developing cardio issues.A systolic blood pressure of 110 decreases your risk age by 13.25 years. A diastolic blood pressure of 80 implies no significant effect of developing cardio issues.A diastolic blood pressure of 80 decreases your risk age by 0.01 years. Having normal cholesterol levels implies no significant effect of developing cardio issues. Having normal cholesterol levels increases your risk age by 9.85 years. Having normal glucose levels implies no significant effect of developing cardio issues. Having normal glucose levels decreases your risk age by 1.92 years. Not smoking implies no significant effect of developing cardio issues. Not smoking decreases your risk age by 2.57 years. Not drinking alcohol implies no significant effect of developing cardio issues. Not drinking alcohol decreases your risk age by 3.49 years. Having an active lifestyle implies no significant effect of developing cardio issues. Having an active lifestyle decreases your risk age by 3.42 years. The patient's overall risk of developing cardio issues is moderately reduced compared to other patients who come into the clinic. The patient's risk of developing cardio issues is equivalent to that of a 33 year old.</t>
   </si>
   <si>
-    <t>An age of 48 implies a moderately reduced risk of developing cardio issues. Being male implies no significant effect of developing cardio issues.A body mass index of 28.71 implies no significant effect of developing cardio issues.A systolic blood pressure of 150 implies a moderately increased risk of developing cardio issues.A diastolic blood pressure of 100 implies a strongly increased risk of developing cardio issues. Having normal cholestero levels implies a strongly reduced risk of developing cardio issues. Having normal glucose levels implies a moderately reduced risk of developing cardio issues. Not smoking implies a moderately reduced risk of developing cardio issues. Not drinking alcohol implies a strongly reduced risk of developing cardio issues. Having an active lifestyle implies a strongly reduced risk of developing cardio issues. The patient's overall risk of developing cardio issues is moderately increased compared to other patients who come into the clinic.</t>
+    <t>Hi! Based on your health data, your overall cardiovascular risk is moderately low, it’s like having the heart health of a typical 33-year-old. Your systolic blood pressure of 110 mmHg is excellent and is a strong protective factor that significantly lowers your risk. Your healthy body mass index (BMI) of 21.97 also helps reduce your chances of heart disease. Good job maintaining normal blood sugar levels, not smoking or drinking alcohol, and staying active, all of these are important ways you’re protecting your heart. That said, even though your cholesterol is reported as “normal,” it’s actually contributing to a higher risk than expected. This means we should look more closely at your lipid profile because some hidden cholesterol factors might increase your risk. Also, being male adds a small extra risk, which is common. To keep your heart healthy, continue controlling your blood pressure, stay active, and avoid smoking and alcohol. We should also talk about your cholesterol to see if changes in diet or medications could help lower your risk further.</t>
   </si>
   <si>
-    <t>An age of 61 implies a moderately increased risk of developing cardio issues. Being female implies a strongly reduced risk of developing cardio issues.A body mass index of 37.73 implies a strongly increased risk of developing cardio issues.A systolic blood pressure of 130 implies no significant effect of developing cardio issues.A diastolic blood pressure of 80 implies a moderately reduced risk of developing cardio issues. Having well above normal cholestero levels implies a moderately increased risk of developing cardio issues. Having normal glucose levels implies a moderately reduced risk of developing cardio issues. Not smoking implies a moderately reduced risk of developing cardio issues. Not drinking alcohol implies a strongly reduced risk of developing cardio issues. Having an active lifestyle implies a strongly reduced risk of developing cardio issues. The patient's overall risk of developing cardio issues is strongly increased compared to other patients who come into the clinic.</t>
+    <t>Hello! You’re doing well overall in terms of heart health. Your age of 50 actually lowers your risk compared to most people your age, and your healthy BMI and excellent systolic blood pressure (110 mmHg) are powerful shields against cardiovascular disease. Keeping normal blood sugar and leading an active lifestyle are additional bonuses that reduce your risk even more. Not smoking and avoiding alcohol also add protection. One point to watch is your cholesterol, although it’s marked as normal, it’s linked to a higher risk in your case. This suggests that some cholesterol components might be hiding risk, so it’s a good idea to check this more thoroughly with your doctor. Your being male adds a little more risk, but overall, your heart age is younger than your actual age. Keep up your healthy habits and consider evaluating your cholesterol in more detail to stay on the right track.</t>
   </si>
   <si>
-    <t>Based on your health metrics, your overall risk of developing cardiovascular issues is average compared to other patients who visit the clinic. Several factors contribute positively to your cardiovascular health, including your age of 46, which moderately reduces your risk, and your normal cholesterol and glucose levels, which strongly and moderately reduce your risk, respectively. Additionally, not smoking and not drinking alcohol further lower your risk, with alcohol abstinence having a particularly strong protective effect. Your blood pressure is also within a range that moderately reduces risk, with a systolic reading of 120 and a diastolic reading of 80. However, certain factors increase your risk, such as a body mass index (BMI) of 37.86, which strongly raises the likelihood of cardiovascular issues, and a lack of physical activity, which moderately increases your risk. Being male does not significantly affect your risk in this context. Overall, while you have several protective factors in your favor, focusing on lowering your BMI and increasing physical activity could greatly improve your cardiovascular health in the future.</t>
+    <t>An age of 50 decreases your risk of developing cardio issues by 17.7% compared to the average patient typically has an average value of 53.7. Being male increases your risk of developing cardio issues by 18.7% compared to the average patient who is female. This corresponds to a 1.61 years increase in risk age. A body mass index of 21.97 decreases your risk of developing cardio issues by 17.5% compared to the average patient typically has an average value of 27.9. This corresponds to a 3.6 years decrease in risk age. A systolic blood pressure of 110 decreases your risk of developing cardio issues by 50.6% compared to the average patient typically has an average value of 128.4. This corresponds to a 13.25 years decrease in risk age. A diastolic blood pressure of 80 decreases your risk of developing cardio issues by 0.0% compared to the average patient typically has an average value of 81.6. This corresponds to a 0.01 years decrease in risk age. Having normal cholesterol levels increases your risk of developing cardio issues by 69.0% compared to the average patient who has normal cholesterol levels. This corresponds to a 9.85 years increase in risk age. Having normal glucose levels decreases your risk of developing cardio issues by 9.7% compared to the average patient who has normal glucose levels. This corresponds to a 1.92 years decrease in risk age. Not smoking does not significantly affect your risk of developing cardio issues.This corresponds to a 2.57 years decrease in risk age. Not drinking alcohol does not significantly affect your risk of developing cardio issues.This corresponds to a 3.49 years decrease in risk age. Having an active lifestyle decreases your risk of developing cardio issues by 16.7% compared to the average patient who has an active lifestyle. This corresponds to a 3.42 years decrease in risk age. The patient's overall risk of developing cardio issues is moderately reduced compared to other patients who come into the clinic. The patient's risk of developing cardio issues is equivalent to that of a 33 year old.</t>
   </si>
   <si>
-    <t>Based on your health metrics, your overall risk of developing cardiovascular issues is moderately increased compared to other patients who visit the clinic. Your age of 48 contributes positively, moderately reducing your risk, while your normal cholesterol and glucose levels further reduce your risk, with cholesterol having a particularly strong effect. Additionally, not smoking, not drinking alcohol and maintaining an active lifestyle strongly reduces your risk factor. However, some factors increase your cardiovascular risk, including a systolic blood pressure of 150, which moderately raises your risk, and a diastolic blood pressure of 100, which strongly increases your risk. Being male and having a body mass index (BMI) of 28.71 have no significant effect on your risk in this context. To lower your overall risk, managing blood pressure levels could be particularly beneficial.</t>
+    <t>Hi there! Your current health data suggest that your cardiovascular risk is moderately increased, similar to someone who is 69 years old, even though you are 52. Your cholesterol levels are the biggest concern here, they are well above normal and significantly increase your heart risk. This is the primary factor driving your elevated risk age. On the bright side, your BMI is within a healthy range, and you have normal blood sugar levels. Avoiding smoking and alcohol also helps lower your risk. Your systolic blood pressure is a bit elevated at 130 mmHg, which slightly increases your risk. To reduce your chances of developing heart disease, focusing on lowering your cholesterol is critical. This can be through lifestyle changes like diet and exercise, and possibly medication. Managing your blood pressure and maintaining your healthy weight will also support your heart health.</t>
   </si>
   <si>
-    <t>Based on your health metrics, your overall risk of developing cardiovascular issues is strongly increased compared to other patients who visit the clinic. Your age of 61 contributes to a moderately increased risk, and your body mass index (BMI) of 37.73 strongly raises your risk. Additionally, having cholesterol levels well above normal further increases your risk moderately. However, several factors contribute positively to your cardiovascular health. Being female strongly reduces your risk, and having normal glucose levels, not smoking, and maintaining a diastolic blood pressure of 80 all moderately reduce your risk. Not drinking alcohol and maintaining an active lifestyle also strongly lower your risk. Your systolic blood pressure of 130 has no significant effect on your risk in this context. To reduce your overall cardiovascular risk, focusing on managing BMI and cholesterol levels could make a significant difference.</t>
+    <t>An age of 52 implies no significant effect of developing cardio issues. Being female implies no significant effect of developing cardio issues. Being female increases your risk age by 1.61 years. A body mass index of 23.51 implies no significant effect of developing cardio issues.A body mass index of 23.51 decreases your risk age by 2.67 years. A systolic blood pressure of 130 implies no significant effect of developing cardio issues.A systolic blood pressure of 130 increases your risk age by 1.16 years. A diastolic blood pressure of 70 implies no significant effect of developing cardio issues.A diastolic blood pressure of 70 decreases your risk age by 0.06 years. Having well above normal cholestero levels implies a strongly increased risk of developing cardio issues. Having well above normal cholestero levels increases your risk age by 9.85 years. Having normal glucose levels implies no significant effect of developing cardio issues. Having normal glucose levels decreases your risk age by 1.92 years. Not smoking implies no significant effect of developing cardio issues. Not smoking decreases your risk age by 2.57 years. Not drinking alcohol implies no significant effect of developing cardio issues. Not drinking alcohol decreases your risk age by 3.49 years. Not having an active lifestyle implies no significant effect of developing cardio issues. Not having an active lifestyle decreases your risk age by 3.42 years. The patient's overall risk of developing cardio issues is moderately increased compared to other patients who come into the clinic. The highest contribution factor for developing cardio issues is the patient's cholesterol. The patient's risk of developing cardio issues is equivalent to that of a 69 year old.</t>
+  </si>
+  <si>
+    <t>Hello! Your cardiovascular risk is moderately higher than average, comparable to that of a 69-year-old, although you are 52. Positive factors helping your heart health include your age, healthy BMI, normal blood sugar, and good diastolic blood pressure. However, your cholesterol levels are well above normal and represent the largest contributor to your increased risk — it’s dramatically raising your chances of heart problems. Being female and having a systolic blood pressure of 130 mmHg also add some risk. Not smoking, not drinking, and physical activity do not seem to add or reduce risk much here, but they remain important lifestyle choices for overall health. The best next step is to work closely with your doctor to lower your cholesterol, which may involve dietary changes and medication, to improve your heart’s long-term health.</t>
+  </si>
+  <si>
+    <t>An age of 52 decreases your risk of developing cardio issues by 8.5% compared to the average patient typically has an average value of 53.7. Being female increases your risk of developing cardio issues by 8.9% compared to the average patient who is female. This corresponds to a 1.61 years increase in risk age. A body mass index of 23.51 decreases your risk of developing cardio issues by 13.3% compared to the average patient typically has an average value of 27.9. This corresponds to a 2.67 years decrease in risk age. A systolic blood pressure of 130 increases your risk of developing cardio issues by 6.4% compared to the average patient typically has an average value of 128.4. This corresponds to a 1.16 years increase in risk age. A diastolic blood pressure of 70 decreases your risk of developing cardio issues by 0.3% compared to the average patient typically has an average value of 81.6. This corresponds to a 0.06 years decreases in risk age. Having well above normal cholesterol levels increases your risk of developing cardio issues by 382.6% compared to the average patient who has normal cholesterol levels. This corresponds to a 9.85 years increases in risk age. Having normal glucose levels decreases your risk of developing cardio issues by 9.7% compared to the average patient who has normal glucose levels. This corresponds to a 1.92 years decreases in risk age. Not smoking does not significantly affect your risk of developing cardio issues.This corresponds to a 2.57 years decreases in risk age. Not drinking alcohol does not significantly affect your risk of developing cardio issues.This corresponds to a 3.49 years decreases in risk age. Not having an active lifestyle does not significantly affect your risk of developing cardio issues.This corresponds to a 3.42 years decreases in risk age. The patient's overall risk of developing cardio issues is moderately increased compared to other patients who come into the clinic. The highest contribution factor for developing cardio issues is the patient's cholesterol. The patient's risk of developing cardio issues is equivalent to that of a 69 year old.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -73,6 +79,18 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -162,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -183,6 +201,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1317,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B2:B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1356,12 +1380,12 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="288" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1382,12 +1406,12 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="360" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1408,12 +1432,12 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1434,9 +1458,13 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:20" ht="234" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -23348,7 +23376,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>